<commit_message>
Video making Report finished
</commit_message>
<xml_diff>
--- a/Graphs/Test 36 and 41 Comparisons.xlsx
+++ b/Graphs/Test 36 and 41 Comparisons.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harri\OneDrive\Documents\Year 3\Project\LearningGitTracker\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD8C128-CBA4-4E0E-AD0E-2BB867B1A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A91B48-860E-47DC-A853-89C65E8380DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mean Reward" sheetId="2" r:id="rId1"/>
     <sheet name="Episode Length" sheetId="3" r:id="rId2"/>
     <sheet name="Data Test 36 and 41" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -596,6 +608,7 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -617,22 +630,44 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
+              <a:rPr lang="en-GB"/>
               <a:t>Mean Reward Per Episode</a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Complex Level</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t>Test 36 and 41</a:t>
+              <a:t> - RL and IL</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38806010289707205"/>
+          <c:y val="1.2121212121212121E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -666,7 +701,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -684,28 +719,30 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:name>RL</c:name>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Data Test 36 and 41'!$B$2:$B$177</c:f>
@@ -1333,7 +1370,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B19E-4768-B4F4-C5C017C01D9B}"/>
+              <c16:uniqueId val="{00000000-BE9B-4F59-BC6F-667C33852B22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1353,28 +1390,30 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:name>IL</c:name>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Data Test 36 and 41'!$B$2:$B$177</c:f>
@@ -2227,7 +2266,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B19E-4768-B4F4-C5C017C01D9B}"/>
+              <c16:uniqueId val="{00000001-BE9B-4F59-BC6F-667C33852B22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2239,11 +2278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="466098648"/>
-        <c:axId val="466096352"/>
+        <c:axId val="1575807871"/>
+        <c:axId val="1575809951"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="466098648"/>
+        <c:axId val="1575807871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2284,7 +2323,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2298,11 +2337,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Number</a:t>
+                  <a:t>Steps Since</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> of Steps Since Training Start</a:t>
+                  <a:t> Training Start</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -2321,7 +2360,151 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1575809951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1575809951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Reward</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> per Episode</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.0522625155405792E-2"/>
+              <c:y val="0.4085201622524457"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2374,138 +2557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466096352"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="466096352"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Mean Reward</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="466098648"/>
+        <c:crossAx val="1575807871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2519,6 +2571,14 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2532,7 +2592,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2593,6 +2653,7 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2615,25 +2676,51 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Average Length</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> of Episode </a:t>
+              <a:t>Average Length of Episode </a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Complex</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t>Test 36 and 41</a:t>
+              <a:t> Level - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>RL</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> and IL </a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38705220884275826"/>
+          <c:y val="1.2121212121212121E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2667,7 +2754,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2685,28 +2772,30 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:name>RL</c:name>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Data Test 36 and 41'!$J$2:$J$177</c:f>
@@ -3334,7 +3423,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AD9F-49B7-A833-CDF62CFC159A}"/>
+              <c16:uniqueId val="{00000000-BE9B-4F59-BC6F-667C33852B22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3354,28 +3443,30 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:name>IL </c:name>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:prstDash val="solid"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Data Test 36 and 41'!$J$2:$J$177</c:f>
@@ -4228,7 +4319,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AD9F-49B7-A833-CDF62CFC159A}"/>
+              <c16:uniqueId val="{00000001-BE9B-4F59-BC6F-667C33852B22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4240,11 +4331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="463809920"/>
-        <c:axId val="463802048"/>
+        <c:axId val="1575807871"/>
+        <c:axId val="1575809951"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="463809920"/>
+        <c:axId val="1575807871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4285,7 +4376,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4299,12 +4390,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Number</a:t>
+                  <a:t>Steps</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> of Steps Since Training Start</a:t>
+                  <a:t> Since Training Start</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4321,7 +4413,151 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1575809951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1575809951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Length</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of Episode</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.7590821561776392E-2"/>
+              <c:y val="0.40447975821204168"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4374,160 +4610,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="463802048"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="463802048"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Average</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Episode Length</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>(Physics</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Steps)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="463809920"/>
+        <c:crossAx val="1575807871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4541,6 +4624,14 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4554,7 +4645,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4603,10 +4694,13 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -4640,10 +4734,13 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -5723,7 +5820,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5734,7 +5831,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663836" cy="6289110"/>
+    <xdr:ext cx="8663609" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6057,11 +6154,583 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L177"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
       <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>

</xml_diff>